<commit_message>
Feature/mx 2025 use organizational units convenience function (#109)
### PR Context


### Changes

- use convenience function to obtain organizational unit merged ids

---------

Co-authored-by: Janina Esins <esinsj@rki.de>
</commit_message>
<xml_diff>
--- a/assets/raw-data/ff-projects/ff-projects.xlsx
+++ b/assets/raw-data/ff-projects/ff-projects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HesseE\mex-extractors\assets\raw-data\ff-projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E32170-58A3-4144-B863-3D19A7FA5838}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D167A614-9A41-4386-AE99-21F5B64B8DD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="15360" windowHeight="4080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t xml:space="preserve">OE without Projektleiter </t>
   </si>
   <si>
-    <t>Department</t>
-  </si>
-  <si>
     <t>Stat. test</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>Robert Koch-Institut</t>
+  </si>
+  <si>
+    <t>C1</t>
   </si>
 </sst>
 </file>
@@ -2053,25 +2053,25 @@
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="14" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" style="14" customWidth="1"/>
     <col min="5" max="5" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="2"/>
+    <col min="6" max="6" width="95.453125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="59.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="59.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
@@ -2103,9 +2103,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="26">
         <v>1364</v>
@@ -2114,22 +2114,22 @@
         <v>9</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I2" s="32"/>
       <c r="J2" s="33"/>
     </row>
-    <row r="3" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>8</v>
       </c>
@@ -2147,15 +2147,15 @@
         <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I3" s="32"/>
       <c r="J3" s="33"/>
     </row>
-    <row r="4" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>16</v>
       </c>
@@ -2178,12 +2178,12 @@
         <v>32</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I4" s="32"/>
       <c r="J4" s="33"/>
     </row>
-    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>11</v>
       </c>
@@ -2204,12 +2204,12 @@
         <v>32</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I5" s="32"/>
       <c r="J5" s="33"/>
     </row>
-    <row r="6" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>11</v>
       </c>
@@ -2224,18 +2224,18 @@
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I6" s="32"/>
       <c r="J6" s="36"/>
     </row>
-    <row r="7" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>11</v>
       </c>
@@ -2253,10 +2253,10 @@
         <v>23</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I7" s="36" t="s">
         <v>24</v>
@@ -2265,9 +2265,9 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="34">
         <v>1364</v>
@@ -2286,7 +2286,7 @@
         <v>32</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I8" s="6">
         <v>43101</v>
@@ -2295,7 +2295,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>11</v>
       </c>
@@ -2310,18 +2310,18 @@
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I9" s="36"/>
       <c r="J9" s="37"/>
     </row>
-    <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>11</v>
       </c>
@@ -2342,12 +2342,12 @@
         <v>40</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I10" s="36"/>
       <c r="J10" s="37"/>
     </row>
-    <row r="11" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>16</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I11" s="6">
         <v>43101</v>
@@ -2379,7 +2379,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25"/>
       <c r="B12" s="34">
         <v>1364</v>
@@ -2398,12 +2398,12 @@
         <v>32</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I12" s="36"/>
       <c r="J12" s="39"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>11</v>
       </c>
@@ -2424,12 +2424,12 @@
         <v>32</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I13" s="36"/>
       <c r="J13" s="39"/>
     </row>
-    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>11</v>
       </c>
@@ -2450,12 +2450,12 @@
         <v>32</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I14" s="36"/>
       <c r="J14" s="39"/>
     </row>
-    <row r="15" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>11</v>
       </c>
@@ -2476,12 +2476,12 @@
         <v>40</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I15" s="36"/>
       <c r="J15" s="39"/>
     </row>
-    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>11</v>
       </c>
@@ -2502,12 +2502,12 @@
         <v>32</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I16" s="36"/>
       <c r="J16" s="39"/>
     </row>
-    <row r="17" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>16</v>
       </c>
@@ -2528,12 +2528,12 @@
         <v>32</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I17" s="40"/>
       <c r="J17" s="37"/>
     </row>
-    <row r="18" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>11</v>
       </c>
@@ -2551,15 +2551,15 @@
         <v>48</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I18" s="40"/>
       <c r="J18" s="37"/>
     </row>
-    <row r="19" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>16</v>
       </c>
@@ -2570,22 +2570,22 @@
         <v>25</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="35"/>
       <c r="F19" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="H19" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I19" s="40"/>
       <c r="J19" s="37"/>
     </row>
-    <row r="20" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
       <c r="B20" s="34">
         <v>1364</v>
@@ -2594,22 +2594,22 @@
         <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I20" s="36"/>
       <c r="J20" s="39"/>
     </row>
-    <row r="21" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
       <c r="B21" s="34">
         <v>1364</v>
@@ -2622,20 +2622,20 @@
       </c>
       <c r="E21" s="35"/>
       <c r="F21" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I21" s="6">
         <v>25204</v>
       </c>
       <c r="J21" s="39"/>
     </row>
-    <row r="22" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
       <c r="B22" s="34">
         <v>1364</v>
@@ -2644,31 +2644,31 @@
         <v>28</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="35"/>
       <c r="F22" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I22" s="36"/>
       <c r="J22" s="6">
         <v>25508</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="7"/>
       <c r="C30" s="12"/>
@@ -2692,16 +2692,16 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:22" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:22" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
@@ -2713,24 +2713,24 @@
       <c r="U40" s="10"/>
       <c r="V40" s="10"/>
     </row>
-    <row r="41" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="13:22" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="13:22" ht="41.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M58" s="10"/>
       <c r="N58" s="10"/>
       <c r="O58" s="10"/>
@@ -2742,10 +2742,10 @@
       <c r="U58" s="10"/>
       <c r="V58" s="10"/>
     </row>
-    <row r="59" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M62" s="10"/>
       <c r="N62" s="10"/>
       <c r="O62" s="10"/>
@@ -2757,7 +2757,7 @@
       <c r="U62" s="10"/>
       <c r="V62" s="10"/>
     </row>
-    <row r="63" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M63" s="10"/>
       <c r="N63" s="10"/>
       <c r="O63" s="10"/>
@@ -2769,7 +2769,7 @@
       <c r="U63" s="10"/>
       <c r="V63" s="10"/>
     </row>
-    <row r="64" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
       <c r="O64" s="10"/>
@@ -2781,20 +2781,20 @@
       <c r="U64" s="10"/>
       <c r="V64" s="10"/>
     </row>
-    <row r="65" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="13:22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="13:22" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="13:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="13:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="13:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="13:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="13:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="13:22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="13:22" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="13:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="13:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="13:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="13:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="13:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M78" s="10"/>
       <c r="N78" s="10"/>
       <c r="O78" s="10"/>
@@ -2806,23 +2806,23 @@
       <c r="U78" s="10"/>
       <c r="V78" s="10"/>
     </row>
-    <row r="79" spans="13:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" spans="13:22" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="13:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="13:22" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M95" s="10"/>
       <c r="N95" s="10"/>
       <c r="O95" s="10"/>
@@ -2834,7 +2834,7 @@
       <c r="U95" s="10"/>
       <c r="V95" s="10"/>
     </row>
-    <row r="96" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
       <c r="O96" s="10"/>
@@ -2846,12 +2846,12 @@
       <c r="U96" s="10"/>
       <c r="V96" s="10"/>
     </row>
-    <row r="97" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" spans="1:22" s="10" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:22" s="10" customFormat="1" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="14"/>
       <c r="B102" s="7"/>
       <c r="C102" s="12"/>
@@ -2875,8 +2875,8 @@
       <c r="U102" s="2"/>
       <c r="V102" s="2"/>
     </row>
-    <row r="103" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" spans="1:22" s="10" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:22" s="10" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="14"/>
       <c r="B104" s="7"/>
       <c r="C104" s="12"/>
@@ -2900,19 +2900,19 @@
       <c r="U104" s="2"/>
       <c r="V104" s="2"/>
     </row>
-    <row r="105" spans="1:22" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:22" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="1:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M117" s="10"/>
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
@@ -2924,25 +2924,25 @@
       <c r="U117" s="10"/>
       <c r="V117" s="10"/>
     </row>
-    <row r="118" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" spans="1:22" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" spans="1:22" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="14"/>
       <c r="B136" s="7"/>
       <c r="D136" s="14"/>
@@ -2965,19 +2965,19 @@
       <c r="U136" s="2"/>
       <c r="V136" s="2"/>
     </row>
-    <row r="137" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M149" s="10"/>
       <c r="N149" s="10"/>
       <c r="O149" s="10"/>
@@ -2989,16 +2989,16 @@
       <c r="U149" s="10"/>
       <c r="V149" s="10"/>
     </row>
-    <row r="150" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" spans="1:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" spans="1:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="14"/>
       <c r="B159" s="7"/>
       <c r="C159" s="12"/>
@@ -3022,27 +3022,27 @@
       <c r="U159" s="2"/>
       <c r="V159" s="2"/>
     </row>
-    <row r="160" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" spans="13:22" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" spans="13:22" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:22" ht="25.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" spans="13:22" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" spans="13:22" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M180" s="10"/>
       <c r="N180" s="10"/>
       <c r="O180" s="10"/>
@@ -3054,7 +3054,7 @@
       <c r="U180" s="10"/>
       <c r="V180" s="10"/>
     </row>
-    <row r="181" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M181" s="10"/>
       <c r="N181" s="10"/>
       <c r="O181" s="10"/>
@@ -3066,18 +3066,18 @@
       <c r="U181" s="10"/>
       <c r="V181" s="10"/>
     </row>
-    <row r="182" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" spans="13:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" spans="13:22" ht="47.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="183" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="186" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" spans="13:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" spans="13:22" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M193" s="13"/>
       <c r="N193" s="13"/>
       <c r="O193" s="13"/>
@@ -3089,11 +3089,11 @@
       <c r="U193" s="13"/>
       <c r="V193" s="13"/>
     </row>
-    <row r="194" spans="13:22" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="13:22" ht="38.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M198" s="10"/>
       <c r="N198" s="10"/>
       <c r="O198" s="10"/>
@@ -3105,29 +3105,29 @@
       <c r="U198" s="10"/>
       <c r="V198" s="10"/>
     </row>
-    <row r="199" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" spans="13:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" spans="13:22" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" spans="13:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" spans="13:22" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M221" s="10"/>
       <c r="N221" s="10"/>
       <c r="O221" s="10"/>
@@ -3139,12 +3139,12 @@
       <c r="U221" s="10"/>
       <c r="V221" s="10"/>
     </row>
-    <row r="222" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" spans="13:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" spans="13:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M227" s="10"/>
       <c r="N227" s="10"/>
       <c r="O227" s="10"/>
@@ -3156,7 +3156,7 @@
       <c r="U227" s="10"/>
       <c r="V227" s="10"/>
     </row>
-    <row r="228" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M228" s="10"/>
       <c r="N228" s="10"/>
       <c r="O228" s="10"/>
@@ -3168,41 +3168,41 @@
       <c r="U228" s="10"/>
       <c r="V228" s="10"/>
     </row>
-    <row r="229" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" spans="13:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" spans="13:22" ht="44.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" spans="13:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" spans="13:22" ht="44.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="239" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M263" s="10"/>
       <c r="N263" s="10"/>
       <c r="O263" s="10"/>
@@ -3214,7 +3214,7 @@
       <c r="U263" s="10"/>
       <c r="V263" s="10"/>
     </row>
-    <row r="264" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M264" s="10"/>
       <c r="N264" s="10"/>
       <c r="O264" s="10"/>
@@ -3226,9 +3226,9 @@
       <c r="U264" s="10"/>
       <c r="V264" s="10"/>
     </row>
-    <row r="265" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" spans="13:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" spans="13:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M267" s="10"/>
       <c r="N267" s="10"/>
       <c r="O267" s="10"/>
@@ -3240,13 +3240,13 @@
       <c r="U267" s="10"/>
       <c r="V267" s="10"/>
     </row>
-    <row r="268" spans="13:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" spans="13:22" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="13:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" spans="13:22" ht="51" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M274" s="10"/>
       <c r="N274" s="10"/>
       <c r="O274" s="10"/>
@@ -3258,9 +3258,9 @@
       <c r="U274" s="10"/>
       <c r="V274" s="10"/>
     </row>
-    <row r="275" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M277" s="10"/>
       <c r="N277" s="10"/>
       <c r="O277" s="10"/>
@@ -3272,9 +3272,9 @@
       <c r="U277" s="10"/>
       <c r="V277" s="10"/>
     </row>
-    <row r="278" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" spans="1:22" s="9" customFormat="1" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" spans="1:22" s="9" customFormat="1" ht="26.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="14"/>
       <c r="B280" s="7"/>
       <c r="C280" s="12"/>
@@ -3298,14 +3298,14 @@
       <c r="U280" s="2"/>
       <c r="V280" s="2"/>
     </row>
-    <row r="281" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" spans="1:22" s="13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" spans="1:22" s="13" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="14"/>
       <c r="B288" s="7"/>
       <c r="C288" s="12"/>
@@ -3329,10 +3329,10 @@
       <c r="U288" s="2"/>
       <c r="V288" s="2"/>
     </row>
-    <row r="289" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M292" s="10"/>
       <c r="N292" s="10"/>
       <c r="O292" s="10"/>
@@ -3344,9 +3344,9 @@
       <c r="U292" s="10"/>
       <c r="V292" s="10"/>
     </row>
-    <row r="293" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M295" s="10"/>
       <c r="N295" s="10"/>
       <c r="O295" s="10"/>
@@ -3358,9 +3358,9 @@
       <c r="U295" s="10"/>
       <c r="V295" s="10"/>
     </row>
-    <row r="296" spans="13:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="13:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M298" s="10"/>
       <c r="N298" s="10"/>
       <c r="O298" s="10"/>
@@ -3372,14 +3372,14 @@
       <c r="U298" s="10"/>
       <c r="V298" s="10"/>
     </row>
-    <row r="299" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M306" s="10"/>
       <c r="N306" s="10"/>
       <c r="O306" s="10"/>
@@ -3391,30 +3391,30 @@
       <c r="U306" s="10"/>
       <c r="V306" s="10"/>
     </row>
-    <row r="307" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" spans="13:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" spans="13:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" spans="13:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" spans="13:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M330" s="10"/>
       <c r="N330" s="10"/>
       <c r="O330" s="10"/>
@@ -3426,9 +3426,9 @@
       <c r="U330" s="10"/>
       <c r="V330" s="10"/>
     </row>
-    <row r="331" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M333" s="10"/>
       <c r="N333" s="10"/>
       <c r="O333" s="10"/>
@@ -3440,8 +3440,8 @@
       <c r="U333" s="10"/>
       <c r="V333" s="10"/>
     </row>
-    <row r="334" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M335" s="10"/>
       <c r="N335" s="10"/>
       <c r="O335" s="10"/>
@@ -3453,7 +3453,7 @@
       <c r="U335" s="10"/>
       <c r="V335" s="10"/>
     </row>
-    <row r="336" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M336" s="10"/>
       <c r="N336" s="10"/>
       <c r="O336" s="10"/>
@@ -3465,7 +3465,7 @@
       <c r="U336" s="10"/>
       <c r="V336" s="10"/>
     </row>
-    <row r="337" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M337" s="10"/>
       <c r="N337" s="10"/>
       <c r="O337" s="10"/>
@@ -3477,8 +3477,8 @@
       <c r="U337" s="10"/>
       <c r="V337" s="10"/>
     </row>
-    <row r="338" spans="1:22" ht="62.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" spans="1:22" s="12" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:22" ht="62.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" spans="1:22" s="12" customFormat="1" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" s="14"/>
       <c r="B339" s="7"/>
       <c r="D339" s="14"/>
@@ -3501,24 +3501,24 @@
       <c r="U339" s="2"/>
       <c r="V339" s="2"/>
     </row>
-    <row r="340" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" spans="1:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M357" s="10"/>
       <c r="N357" s="10"/>
       <c r="O357" s="10"/>
@@ -3530,8 +3530,8 @@
       <c r="U357" s="10"/>
       <c r="V357" s="10"/>
     </row>
-    <row r="358" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M359" s="10"/>
       <c r="N359" s="10"/>
       <c r="O359" s="10"/>
@@ -3543,13 +3543,13 @@
       <c r="U359" s="10"/>
       <c r="V359" s="10"/>
     </row>
-    <row r="360" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M366" s="10"/>
       <c r="N366" s="10"/>
       <c r="O366" s="10"/>
@@ -3561,19 +3561,19 @@
       <c r="U366" s="10"/>
       <c r="V366" s="10"/>
     </row>
-    <row r="367" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M379" s="10"/>
       <c r="N379" s="10"/>
       <c r="O379" s="10"/>
@@ -3585,7 +3585,7 @@
       <c r="U379" s="10"/>
       <c r="V379" s="10"/>
     </row>
-    <row r="380" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M380" s="10"/>
       <c r="N380" s="10"/>
       <c r="O380" s="10"/>
@@ -3597,8 +3597,8 @@
       <c r="U380" s="10"/>
       <c r="V380" s="10"/>
     </row>
-    <row r="381" spans="13:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="13:22" ht="72" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M382" s="10"/>
       <c r="N382" s="10"/>
       <c r="O382" s="10"/>
@@ -3610,8 +3610,8 @@
       <c r="U382" s="10"/>
       <c r="V382" s="10"/>
     </row>
-    <row r="383" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M384" s="10"/>
       <c r="N384" s="10"/>
       <c r="O384" s="10"/>
@@ -3623,7 +3623,7 @@
       <c r="U384" s="10"/>
       <c r="V384" s="10"/>
     </row>
-    <row r="385" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="13:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M385" s="10"/>
       <c r="N385" s="10"/>
       <c r="O385" s="10"/>
@@ -3635,12 +3635,12 @@
       <c r="U385" s="10"/>
       <c r="V385" s="10"/>
     </row>
-    <row r="386" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M391" s="10"/>
       <c r="N391" s="10"/>
       <c r="O391" s="10"/>
@@ -3652,29 +3652,29 @@
       <c r="U391" s="10"/>
       <c r="V391" s="10"/>
     </row>
-    <row r="392" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" spans="13:22" ht="61.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" spans="13:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" spans="13:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" spans="13:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" spans="13:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="13:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" spans="13:22" ht="61.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" spans="13:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" spans="13:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" spans="13:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" spans="13:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M414" s="10"/>
       <c r="N414" s="10"/>
       <c r="O414" s="10"/>
@@ -3686,23 +3686,23 @@
       <c r="U414" s="10"/>
       <c r="V414" s="10"/>
     </row>
-    <row r="415" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" spans="13:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" spans="13:22" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" spans="13:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" spans="13:22" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M431" s="10"/>
       <c r="N431" s="10"/>
       <c r="O431" s="10"/>
@@ -3714,7 +3714,7 @@
       <c r="U431" s="10"/>
       <c r="V431" s="10"/>
     </row>
-    <row r="432" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M432" s="10"/>
       <c r="N432" s="10"/>
       <c r="O432" s="10"/>
@@ -3726,7 +3726,7 @@
       <c r="U432" s="10"/>
       <c r="V432" s="10"/>
     </row>
-    <row r="433" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M433" s="10"/>
       <c r="N433" s="10"/>
       <c r="O433" s="10"/>
@@ -3738,12 +3738,12 @@
       <c r="U433" s="10"/>
       <c r="V433" s="10"/>
     </row>
-    <row r="434" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="434" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M439" s="10"/>
       <c r="N439" s="10"/>
       <c r="O439" s="10"/>
@@ -3755,8 +3755,8 @@
       <c r="U439" s="10"/>
       <c r="V439" s="10"/>
     </row>
-    <row r="440" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" spans="13:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="440" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" spans="13:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M441" s="10"/>
       <c r="N441" s="10"/>
       <c r="O441" s="10"/>
@@ -3768,7 +3768,7 @@
       <c r="U441" s="10"/>
       <c r="V441" s="10"/>
     </row>
-    <row r="442" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="442" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M442" s="10"/>
       <c r="N442" s="10"/>
       <c r="O442" s="10"/>
@@ -3780,8 +3780,8 @@
       <c r="U442" s="10"/>
       <c r="V442" s="10"/>
     </row>
-    <row r="443" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="443" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M444" s="10"/>
       <c r="N444" s="10"/>
       <c r="O444" s="10"/>
@@ -3793,7 +3793,7 @@
       <c r="U444" s="10"/>
       <c r="V444" s="10"/>
     </row>
-    <row r="445" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="445" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M445" s="10"/>
       <c r="N445" s="10"/>
       <c r="O445" s="10"/>
@@ -3805,10 +3805,10 @@
       <c r="U445" s="10"/>
       <c r="V445" s="10"/>
     </row>
-    <row r="446" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="446" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M449" s="10"/>
       <c r="N449" s="10"/>
       <c r="O449" s="10"/>
@@ -3820,10 +3820,10 @@
       <c r="U449" s="10"/>
       <c r="V449" s="10"/>
     </row>
-    <row r="450" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M453" s="10"/>
       <c r="N453" s="10"/>
       <c r="O453" s="10"/>
@@ -3835,9 +3835,9 @@
       <c r="U453" s="10"/>
       <c r="V453" s="10"/>
     </row>
-    <row r="454" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M456" s="10"/>
       <c r="N456" s="10"/>
       <c r="O456" s="10"/>
@@ -3849,7 +3849,7 @@
       <c r="U456" s="10"/>
       <c r="V456" s="10"/>
     </row>
-    <row r="457" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M457" s="10"/>
       <c r="N457" s="10"/>
       <c r="O457" s="10"/>
@@ -3861,11 +3861,11 @@
       <c r="U457" s="10"/>
       <c r="V457" s="10"/>
     </row>
-    <row r="458" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M462" s="10"/>
       <c r="N462" s="10"/>
       <c r="O462" s="10"/>
@@ -3877,11 +3877,11 @@
       <c r="U462" s="10"/>
       <c r="V462" s="10"/>
     </row>
-    <row r="463" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" spans="13:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" spans="13:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M467" s="10"/>
       <c r="N467" s="10"/>
       <c r="O467" s="10"/>
@@ -3893,9 +3893,9 @@
       <c r="U467" s="10"/>
       <c r="V467" s="10"/>
     </row>
-    <row r="468" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M470" s="10"/>
       <c r="N470" s="10"/>
       <c r="O470" s="10"/>
@@ -3907,13 +3907,13 @@
       <c r="U470" s="10"/>
       <c r="V470" s="10"/>
     </row>
-    <row r="471" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" spans="13:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" spans="13:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" spans="13:22" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="471" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" spans="13:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" spans="13:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" spans="13:22" ht="23.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M477" s="10"/>
       <c r="N477" s="10"/>
       <c r="O477" s="10"/>
@@ -3925,7 +3925,7 @@
       <c r="U477" s="10"/>
       <c r="V477" s="10"/>
     </row>
-    <row r="478" spans="13:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="13:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M478" s="10"/>
       <c r="N478" s="10"/>
       <c r="O478" s="10"/>
@@ -3937,11 +3937,11 @@
       <c r="U478" s="10"/>
       <c r="V478" s="10"/>
     </row>
-    <row r="479" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M483" s="10"/>
       <c r="N483" s="10"/>
       <c r="O483" s="10"/>
@@ -3953,9 +3953,9 @@
       <c r="U483" s="10"/>
       <c r="V483" s="10"/>
     </row>
-    <row r="484" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M486" s="10"/>
       <c r="N486" s="10"/>
       <c r="O486" s="10"/>
@@ -3967,8 +3967,8 @@
       <c r="U486" s="10"/>
       <c r="V486" s="10"/>
     </row>
-    <row r="487" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M488" s="10"/>
       <c r="N488" s="10"/>
       <c r="O488" s="10"/>
@@ -3980,12 +3980,12 @@
       <c r="U488" s="10"/>
       <c r="V488" s="10"/>
     </row>
-    <row r="489" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" spans="1:22" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" spans="1:22" s="10" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" spans="1:22" ht="63.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" spans="1:22" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A494" s="14"/>
       <c r="B494" s="7"/>
       <c r="C494" s="12"/>
@@ -4009,20 +4009,20 @@
       <c r="U494" s="2"/>
       <c r="V494" s="2"/>
     </row>
-    <row r="495" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" spans="1:22" ht="59.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" spans="1:22" ht="59.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M508" s="10"/>
       <c r="N508" s="10"/>
       <c r="O508" s="10"/>
@@ -4034,10 +4034,10 @@
       <c r="U508" s="10"/>
       <c r="V508" s="10"/>
     </row>
-    <row r="509" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A512" s="14"/>
       <c r="B512" s="7"/>
       <c r="C512" s="12"/>
@@ -4061,9 +4061,9 @@
       <c r="U512" s="2"/>
       <c r="V512" s="2"/>
     </row>
-    <row r="513" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M515" s="10"/>
       <c r="N515" s="10"/>
       <c r="O515" s="10"/>
@@ -4075,7 +4075,7 @@
       <c r="U515" s="10"/>
       <c r="V515" s="10"/>
     </row>
-    <row r="516" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A516" s="14"/>
       <c r="B516" s="7"/>
       <c r="C516" s="12"/>
@@ -4099,7 +4099,7 @@
       <c r="U516" s="2"/>
       <c r="V516" s="2"/>
     </row>
-    <row r="517" spans="1:22" s="10" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:22" s="10" customFormat="1" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A517" s="14"/>
       <c r="B517" s="7"/>
       <c r="C517" s="12"/>
@@ -4123,7 +4123,7 @@
       <c r="U517" s="2"/>
       <c r="V517" s="2"/>
     </row>
-    <row r="518" spans="1:22" s="10" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:22" s="10" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A518" s="14"/>
       <c r="B518" s="7"/>
       <c r="C518" s="12"/>
@@ -4147,8 +4147,8 @@
       <c r="U518" s="2"/>
       <c r="V518" s="2"/>
     </row>
-    <row r="519" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M520" s="10"/>
       <c r="N520" s="10"/>
       <c r="O520" s="10"/>
@@ -4160,16 +4160,16 @@
       <c r="U520" s="10"/>
       <c r="V520" s="10"/>
     </row>
-    <row r="521" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M530" s="10"/>
       <c r="N530" s="10"/>
       <c r="O530" s="10"/>
@@ -4181,8 +4181,8 @@
       <c r="U530" s="10"/>
       <c r="V530" s="10"/>
     </row>
-    <row r="531" spans="1:22" ht="42.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="531" spans="1:22" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A532" s="14"/>
       <c r="B532" s="7"/>
       <c r="C532" s="12"/>
@@ -4206,8 +4206,8 @@
       <c r="U532" s="2"/>
       <c r="V532" s="2"/>
     </row>
-    <row r="533" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M534" s="10"/>
       <c r="N534" s="10"/>
       <c r="O534" s="10"/>
@@ -4219,17 +4219,17 @@
       <c r="U534" s="10"/>
       <c r="V534" s="10"/>
     </row>
-    <row r="535" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" spans="1:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M545" s="10"/>
       <c r="N545" s="10"/>
       <c r="O545" s="10"/>
@@ -4241,10 +4241,10 @@
       <c r="U545" s="10"/>
       <c r="V545" s="10"/>
     </row>
-    <row r="546" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" spans="1:22" s="10" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" spans="1:22" s="10" customFormat="1" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A549" s="14"/>
       <c r="B549" s="7"/>
       <c r="C549" s="12"/>
@@ -4268,7 +4268,7 @@
       <c r="U549" s="2"/>
       <c r="V549" s="2"/>
     </row>
-    <row r="550" spans="1:22" s="10" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:22" s="10" customFormat="1" ht="30.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A550" s="14"/>
       <c r="B550" s="7"/>
       <c r="C550" s="12"/>
@@ -4282,13 +4282,13 @@
       <c r="K550" s="2"/>
       <c r="L550" s="2"/>
     </row>
-    <row r="551" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M557" s="10"/>
       <c r="N557" s="10"/>
       <c r="O557" s="10"/>
@@ -4300,7 +4300,7 @@
       <c r="U557" s="10"/>
       <c r="V557" s="10"/>
     </row>
-    <row r="558" spans="1:22" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:22" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M558" s="10"/>
       <c r="N558" s="10"/>
       <c r="O558" s="10"/>
@@ -4312,16 +4312,16 @@
       <c r="U558" s="10"/>
       <c r="V558" s="10"/>
     </row>
-    <row r="559" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" spans="1:22" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" spans="1:22" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M568" s="10"/>
       <c r="N568" s="10"/>
       <c r="O568" s="10"/>
@@ -4333,7 +4333,7 @@
       <c r="U568" s="10"/>
       <c r="V568" s="10"/>
     </row>
-    <row r="569" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M569" s="10"/>
       <c r="N569" s="10"/>
       <c r="O569" s="10"/>
@@ -4345,8 +4345,8 @@
       <c r="U569" s="10"/>
       <c r="V569" s="10"/>
     </row>
-    <row r="570" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" spans="1:22" s="10" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" spans="1:22" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A571" s="14"/>
       <c r="B571" s="7"/>
       <c r="C571" s="12"/>
@@ -4370,34 +4370,34 @@
       <c r="U571" s="2"/>
       <c r="V571" s="2"/>
     </row>
-    <row r="572" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="39" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" ht="50.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M599" s="10"/>
       <c r="N599" s="10"/>
       <c r="O599" s="10"/>
@@ -4409,7 +4409,7 @@
       <c r="U599" s="10"/>
       <c r="V599" s="10"/>
     </row>
-    <row r="600" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M600" s="10"/>
       <c r="N600" s="10"/>
       <c r="O600" s="10"/>
@@ -4421,9 +4421,9 @@
       <c r="U600" s="10"/>
       <c r="V600" s="10"/>
     </row>
-    <row r="601" spans="1:22" ht="48" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" spans="1:22" s="10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:22" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" spans="1:22" s="10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A603" s="14"/>
       <c r="B603" s="7"/>
       <c r="C603" s="12"/>
@@ -4447,19 +4447,19 @@
       <c r="U603" s="2"/>
       <c r="V603" s="2"/>
     </row>
-    <row r="604" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" spans="13:22" ht="60" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" spans="13:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" spans="13:22" ht="60" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" spans="13:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M616" s="10"/>
       <c r="N616" s="10"/>
       <c r="O616" s="10"/>
@@ -4471,7 +4471,7 @@
       <c r="U616" s="10"/>
       <c r="V616" s="10"/>
     </row>
-    <row r="617" spans="13:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="617" spans="13:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M617" s="10"/>
       <c r="N617" s="10"/>
       <c r="O617" s="10"/>
@@ -4483,14 +4483,14 @@
       <c r="U617" s="10"/>
       <c r="V617" s="10"/>
     </row>
-    <row r="618" spans="13:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" spans="13:22" ht="69" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="13:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" spans="13:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" spans="13:22" ht="69" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M625" s="10"/>
       <c r="N625" s="10"/>
       <c r="O625" s="10"/>
@@ -4502,15 +4502,15 @@
       <c r="U625" s="10"/>
       <c r="V625" s="10"/>
     </row>
-    <row r="626" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A634" s="14"/>
       <c r="B634" s="7"/>
       <c r="C634" s="12"/>
@@ -4534,7 +4534,7 @@
       <c r="U634" s="2"/>
       <c r="V634" s="2"/>
     </row>
-    <row r="635" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A635" s="14"/>
       <c r="B635" s="7"/>
       <c r="C635" s="12"/>
@@ -4558,18 +4558,18 @@
       <c r="U635" s="2"/>
       <c r="V635" s="2"/>
     </row>
-    <row r="636" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" spans="1:22" s="13" customFormat="1" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" spans="1:22" s="13" customFormat="1" ht="26.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A647" s="14"/>
       <c r="B647" s="7"/>
       <c r="C647" s="12"/>
@@ -4593,10 +4593,10 @@
       <c r="U647" s="2"/>
       <c r="V647" s="2"/>
     </row>
-    <row r="648" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" spans="1:22" ht="39.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="648" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" spans="1:22" ht="39.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M651" s="10"/>
       <c r="N651" s="10"/>
       <c r="O651" s="10"/>
@@ -4608,7 +4608,7 @@
       <c r="U651" s="10"/>
       <c r="V651" s="10"/>
     </row>
-    <row r="652" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="652" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A652" s="14"/>
       <c r="B652" s="7"/>
       <c r="C652" s="12"/>
@@ -4622,29 +4622,29 @@
       <c r="K652" s="2"/>
       <c r="L652" s="2"/>
     </row>
-    <row r="653" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" spans="1:22" ht="42.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" spans="1:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" spans="1:22" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="55.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" spans="1:22" ht="83.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" spans="1:22" s="10" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="653" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" spans="1:22" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" spans="1:22" ht="50.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" spans="1:22" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" ht="55.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" ht="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" spans="1:22" ht="83.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" spans="1:22" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A675" s="14"/>
       <c r="B675" s="7"/>
       <c r="C675" s="12"/>
@@ -4668,12 +4668,12 @@
       <c r="U675" s="2"/>
       <c r="V675" s="2"/>
     </row>
-    <row r="676" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" spans="1:22" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="676" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" spans="1:22" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A681" s="14"/>
       <c r="B681" s="7"/>
       <c r="C681" s="12"/>
@@ -4697,7 +4697,7 @@
       <c r="U681" s="2"/>
       <c r="V681" s="2"/>
     </row>
-    <row r="682" spans="1:22" s="10" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="682" spans="1:22" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A682" s="14"/>
       <c r="B682" s="7"/>
       <c r="C682" s="12"/>
@@ -4721,9 +4721,9 @@
       <c r="U682" s="2"/>
       <c r="V682" s="2"/>
     </row>
-    <row r="683" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="683" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M685" s="10"/>
       <c r="N685" s="10"/>
       <c r="O685" s="10"/>
@@ -4735,8 +4735,8 @@
       <c r="U685" s="10"/>
       <c r="V685" s="10"/>
     </row>
-    <row r="686" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="686" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M687" s="10"/>
       <c r="N687" s="10"/>
       <c r="O687" s="10"/>
@@ -4748,10 +4748,10 @@
       <c r="U687" s="10"/>
       <c r="V687" s="10"/>
     </row>
-    <row r="688" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" spans="13:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="688" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" spans="13:22" ht="51.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" spans="13:22" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M691" s="7"/>
       <c r="N691" s="7"/>
       <c r="O691" s="7"/>
@@ -4763,10 +4763,10 @@
       <c r="U691" s="7"/>
       <c r="V691" s="7"/>
     </row>
-    <row r="692" spans="13:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" spans="13:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="692" spans="13:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" spans="13:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M695" s="7"/>
       <c r="N695" s="7"/>
       <c r="O695" s="7"/>
@@ -4778,12 +4778,12 @@
       <c r="U695" s="7"/>
       <c r="V695" s="7"/>
     </row>
-    <row r="696" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" spans="13:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" spans="13:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="696" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" spans="13:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" spans="13:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M701" s="10"/>
       <c r="N701" s="10"/>
       <c r="O701" s="10"/>
@@ -4795,15 +4795,15 @@
       <c r="U701" s="10"/>
       <c r="V701" s="10"/>
     </row>
-    <row r="702" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" spans="13:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="702" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" spans="13:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" spans="13:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M710" s="10"/>
       <c r="N710" s="10"/>
       <c r="O710" s="10"/>
@@ -4815,8 +4815,8 @@
       <c r="U710" s="10"/>
       <c r="V710" s="10"/>
     </row>
-    <row r="711" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" spans="1:22" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="711" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" spans="1:22" ht="23.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M712" s="10"/>
       <c r="N712" s="10"/>
       <c r="O712" s="10"/>
@@ -4828,11 +4828,11 @@
       <c r="U712" s="10"/>
       <c r="V712" s="10"/>
     </row>
-    <row r="713" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="713" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A717" s="14"/>
       <c r="B717" s="7"/>
       <c r="C717" s="12"/>
@@ -4856,7 +4856,7 @@
       <c r="U717" s="17"/>
       <c r="V717" s="17"/>
     </row>
-    <row r="718" spans="1:22" s="10" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="718" spans="1:22" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A718" s="14"/>
       <c r="B718" s="7"/>
       <c r="C718" s="12"/>
@@ -4880,9 +4880,9 @@
       <c r="U718" s="2"/>
       <c r="V718" s="2"/>
     </row>
-    <row r="719" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" spans="1:22" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="719" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" spans="1:22" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A721" s="14"/>
       <c r="B721" s="7"/>
       <c r="C721" s="12"/>
@@ -4906,13 +4906,13 @@
       <c r="U721" s="2"/>
       <c r="V721" s="2"/>
     </row>
-    <row r="722" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="722" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A728" s="14"/>
       <c r="B728" s="7"/>
       <c r="C728" s="12"/>
@@ -4936,9 +4936,9 @@
       <c r="U728" s="2"/>
       <c r="V728" s="2"/>
     </row>
-    <row r="729" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" spans="1:22" s="10" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="729" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" spans="1:22" s="10" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A731" s="14"/>
       <c r="B731" s="7"/>
       <c r="C731" s="12"/>
@@ -4962,20 +4962,20 @@
       <c r="U731" s="2"/>
       <c r="V731" s="2"/>
     </row>
-    <row r="732" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" spans="1:22" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="732" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" spans="1:22" ht="23.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A746" s="14"/>
       <c r="B746" s="7"/>
       <c r="C746" s="12"/>
@@ -4999,9 +4999,9 @@
       <c r="U746" s="2"/>
       <c r="V746" s="2"/>
     </row>
-    <row r="747" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="747" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A749" s="14"/>
       <c r="B749" s="7"/>
       <c r="C749" s="12"/>
@@ -5025,9 +5025,9 @@
       <c r="U749" s="2"/>
       <c r="V749" s="2"/>
     </row>
-    <row r="750" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" spans="1:22" s="10" customFormat="1" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="750" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" spans="1:22" s="10" customFormat="1" ht="26.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A752" s="14"/>
       <c r="B752" s="7"/>
       <c r="C752" s="12"/>
@@ -5051,14 +5051,14 @@
       <c r="U752" s="2"/>
       <c r="V752" s="2"/>
     </row>
-    <row r="753" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="753" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A760" s="14"/>
       <c r="B760" s="7"/>
       <c r="C760" s="12"/>
@@ -5082,30 +5082,30 @@
       <c r="U760" s="2"/>
       <c r="V760" s="2"/>
     </row>
-    <row r="761" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" spans="1:22" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" spans="1:22" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" spans="1:22" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" spans="1:22" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="761" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" spans="1:22" ht="25.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" spans="1:22" ht="25.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" spans="1:22" ht="41.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" spans="1:22" ht="23.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" spans="1:22" ht="23.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" spans="1:22" ht="23.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A784" s="14"/>
       <c r="B784" s="7"/>
       <c r="C784" s="12"/>
@@ -5129,9 +5129,9 @@
       <c r="U784" s="2"/>
       <c r="V784" s="2"/>
     </row>
-    <row r="785" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="785" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A787" s="14"/>
       <c r="B787" s="7"/>
       <c r="C787" s="12"/>
@@ -5155,8 +5155,8 @@
       <c r="U787" s="2"/>
       <c r="V787" s="2"/>
     </row>
-    <row r="788" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="788" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" spans="1:22" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A789" s="14"/>
       <c r="B789" s="7"/>
       <c r="C789" s="12"/>
@@ -5180,7 +5180,7 @@
       <c r="U789" s="2"/>
       <c r="V789" s="2"/>
     </row>
-    <row r="790" spans="1:22" s="10" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="790" spans="1:22" s="10" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A790" s="14"/>
       <c r="B790" s="7"/>
       <c r="C790" s="12"/>
@@ -5204,7 +5204,7 @@
       <c r="U790" s="2"/>
       <c r="V790" s="2"/>
     </row>
-    <row r="791" spans="1:22" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="791" spans="1:22" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A791" s="14"/>
       <c r="B791" s="7"/>
       <c r="C791" s="12"/>
@@ -5228,26 +5228,26 @@
       <c r="U791" s="2"/>
       <c r="V791" s="2"/>
     </row>
-    <row r="792" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" spans="1:22" s="10" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="792" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" spans="1:22" ht="57" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" spans="1:22" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A811" s="14"/>
       <c r="B811" s="7"/>
       <c r="C811" s="12"/>
@@ -5271,8 +5271,8 @@
       <c r="U811" s="2"/>
       <c r="V811" s="2"/>
     </row>
-    <row r="812" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" spans="1:22" s="10" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="812" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" spans="1:22" s="10" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A813" s="14"/>
       <c r="B813" s="7"/>
       <c r="C813" s="12"/>
@@ -5296,13 +5296,13 @@
       <c r="U813" s="2"/>
       <c r="V813" s="2"/>
     </row>
-    <row r="814" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="814" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A820" s="14"/>
       <c r="B820" s="7"/>
       <c r="C820" s="12"/>
@@ -5326,19 +5326,19 @@
       <c r="U820" s="2"/>
       <c r="V820" s="2"/>
     </row>
-    <row r="821" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" spans="1:22" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="821" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" spans="1:22" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A833" s="14"/>
       <c r="B833" s="7"/>
       <c r="C833" s="12"/>
@@ -5362,7 +5362,7 @@
       <c r="U833" s="2"/>
       <c r="V833" s="2"/>
     </row>
-    <row r="834" spans="1:22" s="10" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="834" spans="1:22" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A834" s="14"/>
       <c r="B834" s="7"/>
       <c r="C834" s="12"/>
@@ -5386,8 +5386,8 @@
       <c r="U834" s="2"/>
       <c r="V834" s="2"/>
     </row>
-    <row r="835" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="835" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A836" s="14"/>
       <c r="B836" s="7"/>
       <c r="C836" s="12"/>
@@ -5411,8 +5411,8 @@
       <c r="U836" s="2"/>
       <c r="V836" s="2"/>
     </row>
-    <row r="837" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A838" s="14"/>
       <c r="B838" s="7"/>
       <c r="C838" s="12"/>
@@ -5436,7 +5436,7 @@
       <c r="U838" s="2"/>
       <c r="V838" s="2"/>
     </row>
-    <row r="839" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="839" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A839" s="14"/>
       <c r="B839" s="7"/>
       <c r="C839" s="12"/>
@@ -5460,12 +5460,12 @@
       <c r="U839" s="2"/>
       <c r="V839" s="2"/>
     </row>
-    <row r="840" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="840" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A845" s="14"/>
       <c r="B845" s="7"/>
       <c r="C845" s="12"/>
@@ -5489,29 +5489,29 @@
       <c r="U845" s="2"/>
       <c r="V845" s="2"/>
     </row>
-    <row r="846" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" spans="1:22" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="846" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" ht="41.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" spans="1:22" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A868" s="14"/>
       <c r="B868" s="7"/>
       <c r="C868" s="12"/>
@@ -5535,23 +5535,23 @@
       <c r="U868" s="2"/>
       <c r="V868" s="2"/>
     </row>
-    <row r="869" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" spans="1:22" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="869" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" spans="1:22" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A885" s="14"/>
       <c r="B885" s="7"/>
       <c r="C885" s="12"/>
@@ -5575,7 +5575,7 @@
       <c r="U885" s="2"/>
       <c r="V885" s="2"/>
     </row>
-    <row r="886" spans="1:22" s="10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="886" spans="1:22" s="10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A886" s="14"/>
       <c r="B886" s="7"/>
       <c r="C886" s="12"/>
@@ -5599,7 +5599,7 @@
       <c r="U886" s="2"/>
       <c r="V886" s="2"/>
     </row>
-    <row r="887" spans="1:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="887" spans="1:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A887" s="14"/>
       <c r="B887" s="7"/>
       <c r="C887" s="12"/>
@@ -5623,12 +5623,12 @@
       <c r="U887" s="2"/>
       <c r="V887" s="2"/>
     </row>
-    <row r="888" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" spans="1:22" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" spans="1:22" s="10" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="888" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" spans="1:22" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" spans="1:22" s="10" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A893" s="14"/>
       <c r="B893" s="7"/>
       <c r="C893" s="12"/>
@@ -5652,8 +5652,8 @@
       <c r="U893" s="2"/>
       <c r="V893" s="2"/>
     </row>
-    <row r="894" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" spans="1:22" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="894" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" spans="1:22" s="10" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A895" s="14"/>
       <c r="B895" s="7"/>
       <c r="C895" s="12"/>
@@ -5677,7 +5677,7 @@
       <c r="U895" s="2"/>
       <c r="V895" s="2"/>
     </row>
-    <row r="896" spans="1:22" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="896" spans="1:22" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A896" s="14"/>
       <c r="B896" s="7"/>
       <c r="C896" s="12"/>
@@ -5701,8 +5701,8 @@
       <c r="U896" s="2"/>
       <c r="V896" s="2"/>
     </row>
-    <row r="897" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="897" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A898" s="14"/>
       <c r="B898" s="7"/>
       <c r="C898" s="12"/>
@@ -5726,7 +5726,7 @@
       <c r="U898" s="2"/>
       <c r="V898" s="2"/>
     </row>
-    <row r="899" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="899" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A899" s="14"/>
       <c r="B899" s="7"/>
       <c r="C899" s="12"/>
@@ -5750,10 +5750,10 @@
       <c r="U899" s="2"/>
       <c r="V899" s="2"/>
     </row>
-    <row r="900" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="900" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A903" s="14"/>
       <c r="B903" s="7"/>
       <c r="C903" s="12"/>
@@ -5777,10 +5777,10 @@
       <c r="U903" s="2"/>
       <c r="V903" s="2"/>
     </row>
-    <row r="904" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="904" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A907" s="14"/>
       <c r="B907" s="7"/>
       <c r="C907" s="12"/>
@@ -5804,9 +5804,9 @@
       <c r="U907" s="2"/>
       <c r="V907" s="2"/>
     </row>
-    <row r="908" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" spans="1:22" s="10" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="908" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" spans="1:22" s="10" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A910" s="14"/>
       <c r="B910" s="7"/>
       <c r="C910" s="12"/>
@@ -5830,7 +5830,7 @@
       <c r="U910" s="2"/>
       <c r="V910" s="2"/>
     </row>
-    <row r="911" spans="1:22" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="911" spans="1:22" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A911" s="14"/>
       <c r="B911" s="7"/>
       <c r="C911" s="12"/>
@@ -5854,11 +5854,11 @@
       <c r="U911" s="2"/>
       <c r="V911" s="2"/>
     </row>
-    <row r="912" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="912" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A916" s="14"/>
       <c r="B916" s="7"/>
       <c r="C916" s="12"/>
@@ -5882,11 +5882,11 @@
       <c r="U916" s="2"/>
       <c r="V916" s="2"/>
     </row>
-    <row r="917" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="917" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" spans="1:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A921" s="14"/>
       <c r="B921" s="7"/>
       <c r="C921" s="12"/>
@@ -5910,9 +5910,9 @@
       <c r="U921" s="2"/>
       <c r="V921" s="2"/>
     </row>
-    <row r="922" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="922" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A924" s="14"/>
       <c r="B924" s="7"/>
       <c r="C924" s="12"/>
@@ -5936,13 +5936,13 @@
       <c r="U924" s="2"/>
       <c r="V924" s="2"/>
     </row>
-    <row r="925" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="925" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A931" s="14"/>
       <c r="B931" s="7"/>
       <c r="C931" s="12"/>
@@ -5966,7 +5966,7 @@
       <c r="U931" s="2"/>
       <c r="V931" s="2"/>
     </row>
-    <row r="932" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="932" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A932" s="14"/>
       <c r="B932" s="7"/>
       <c r="C932" s="12"/>
@@ -5990,11 +5990,11 @@
       <c r="U932" s="2"/>
       <c r="V932" s="2"/>
     </row>
-    <row r="933" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" spans="1:22" s="10" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="933" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" spans="1:22" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A937" s="14"/>
       <c r="B937" s="7"/>
       <c r="C937" s="12"/>
@@ -6018,9 +6018,9 @@
       <c r="U937" s="2"/>
       <c r="V937" s="2"/>
     </row>
-    <row r="938" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="938" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A940" s="14"/>
       <c r="B940" s="7"/>
       <c r="C940" s="12"/>
@@ -6044,8 +6044,8 @@
       <c r="U940" s="2"/>
       <c r="V940" s="2"/>
     </row>
-    <row r="941" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="941" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A942" s="14"/>
       <c r="B942" s="7"/>
       <c r="C942" s="12"/>
@@ -6069,26 +6069,26 @@
       <c r="U942" s="2"/>
       <c r="V942" s="2"/>
     </row>
-    <row r="943" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="943" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" ht="23.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" ht="23.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A962" s="14"/>
       <c r="B962" s="7"/>
       <c r="C962" s="12"/>
@@ -6112,13 +6112,13 @@
       <c r="U962" s="2"/>
       <c r="V962" s="2"/>
     </row>
-    <row r="963" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" spans="1:22" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="963" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" spans="1:22" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A969" s="14"/>
       <c r="B969" s="7"/>
       <c r="C969" s="12"/>
@@ -6142,11 +6142,11 @@
       <c r="U969" s="2"/>
       <c r="V969" s="2"/>
     </row>
-    <row r="970" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="970" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A974" s="14"/>
       <c r="B974" s="7"/>
       <c r="C974" s="12"/>
@@ -6170,16 +6170,16 @@
       <c r="U974" s="2"/>
       <c r="V974" s="2"/>
     </row>
-    <row r="975" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" spans="1:22" s="10" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="975" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" spans="1:22" s="10" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A984" s="14"/>
       <c r="B984" s="7"/>
       <c r="C984" s="12"/>
@@ -6203,10 +6203,10 @@
       <c r="U984" s="2"/>
       <c r="V984" s="2"/>
     </row>
-    <row r="985" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" spans="1:22" ht="69" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" spans="1:22" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="985" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" spans="1:22" ht="69" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" spans="1:22" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A988" s="14"/>
       <c r="B988" s="7"/>
       <c r="C988" s="12"/>
@@ -6230,17 +6230,17 @@
       <c r="U988" s="2"/>
       <c r="V988" s="2"/>
     </row>
-    <row r="989" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="989" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A999" s="14"/>
       <c r="B999" s="7"/>
       <c r="C999" s="12"/>
@@ -6264,8 +6264,8 @@
       <c r="U999" s="2"/>
       <c r="V999" s="2"/>
     </row>
-    <row r="1000" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1004" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1000" spans="1:22" ht="14.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1004" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1004" s="14"/>
       <c r="B1004" s="7"/>
       <c r="C1004" s="12"/>
@@ -6289,7 +6289,7 @@
       <c r="U1004" s="2"/>
       <c r="V1004" s="2"/>
     </row>
-    <row r="1011" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1011" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1011" s="14"/>
       <c r="B1011" s="7"/>
       <c r="C1011" s="12"/>
@@ -6313,7 +6313,7 @@
       <c r="U1011" s="2"/>
       <c r="V1011" s="2"/>
     </row>
-    <row r="1012" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1012" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1012" s="14"/>
       <c r="B1012" s="7"/>
       <c r="C1012" s="12"/>
@@ -6337,8 +6337,8 @@
       <c r="U1012" s="2"/>
       <c r="V1012" s="2"/>
     </row>
-    <row r="1020" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1022" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1020" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1022" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1022" s="14"/>
       <c r="B1022" s="7"/>
       <c r="C1022" s="12"/>
@@ -6362,7 +6362,7 @@
       <c r="U1022" s="2"/>
       <c r="V1022" s="2"/>
     </row>
-    <row r="1023" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1023" spans="1:22" s="10" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1023" s="14"/>
       <c r="B1023" s="7"/>
       <c r="C1023" s="12"/>
@@ -6386,17 +6386,17 @@
       <c r="U1023" s="2"/>
       <c r="V1023" s="2"/>
     </row>
-    <row r="1025" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1029" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1033" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1035" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1038" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1039" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1040" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1041" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1042" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1044" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1053" spans="1:22" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1025" ht="21.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1029" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1033" ht="21.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1035" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1038" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1039" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1040" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1041" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1042" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1044" spans="1:22" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1053" spans="1:22" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1053" s="14"/>
       <c r="B1053" s="7"/>
       <c r="C1053" s="12"/>
@@ -6420,7 +6420,7 @@
       <c r="U1053" s="2"/>
       <c r="V1053" s="2"/>
     </row>
-    <row r="1054" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1054" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1054" s="14"/>
       <c r="B1054" s="7"/>
       <c r="C1054" s="12"/>
@@ -6444,7 +6444,7 @@
       <c r="U1054" s="2"/>
       <c r="V1054" s="2"/>
     </row>
-    <row r="1070" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1070" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1070" s="14"/>
       <c r="B1070" s="7"/>
       <c r="C1070" s="12"/>
@@ -6468,7 +6468,7 @@
       <c r="U1070" s="2"/>
       <c r="V1070" s="2"/>
     </row>
-    <row r="1071" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1071" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1071" s="14"/>
       <c r="B1071" s="7"/>
       <c r="C1071" s="12"/>
@@ -6492,7 +6492,7 @@
       <c r="U1071" s="2"/>
       <c r="V1071" s="2"/>
     </row>
-    <row r="1079" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1079" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1079" s="14"/>
       <c r="B1079" s="7"/>
       <c r="C1079" s="12"/>
@@ -6516,8 +6516,8 @@
       <c r="U1079" s="2"/>
       <c r="V1079" s="2"/>
     </row>
-    <row r="1100" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1105" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1100" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1105" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1105" s="14"/>
       <c r="B1105" s="7"/>
       <c r="C1105" s="12"/>
@@ -6541,7 +6541,7 @@
       <c r="U1105" s="2"/>
       <c r="V1105" s="2"/>
     </row>
-    <row r="1106" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1106" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1106" s="14"/>
       <c r="B1106" s="7"/>
       <c r="C1106" s="12"/>
@@ -6565,26 +6565,26 @@
       <c r="U1106" s="2"/>
       <c r="V1106" s="2"/>
     </row>
-    <row r="1114" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1115" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1116" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1117" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1118" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1119" spans="1:22" ht="42.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1120" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1121" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1122" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1123" ht="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1124" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1125" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1126" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1127" ht="47.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1128" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1129" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1130" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1131" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1132" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1139" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1114" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1115" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1116" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1117" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1118" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1119" spans="1:22" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1120" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1121" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1122" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1123" ht="33.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1124" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1125" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1126" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1127" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1128" ht="32.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1129" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1130" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1131" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1132" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1139" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1139" s="14"/>
       <c r="B1139" s="7"/>
       <c r="C1139" s="12"/>
@@ -6608,7 +6608,7 @@
       <c r="U1139" s="2"/>
       <c r="V1139" s="2"/>
     </row>
-    <row r="1141" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1141" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1141" s="14"/>
       <c r="B1141" s="7"/>
       <c r="C1141" s="12"/>
@@ -6632,7 +6632,7 @@
       <c r="U1141" s="2"/>
       <c r="V1141" s="2"/>
     </row>
-    <row r="1145" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1145" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1145" s="14"/>
       <c r="C1145" s="12"/>
       <c r="D1145" s="14"/>
@@ -6655,7 +6655,7 @@
       <c r="U1145" s="2"/>
       <c r="V1145" s="2"/>
     </row>
-    <row r="1149" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1149" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1149" s="14"/>
       <c r="C1149" s="12"/>
       <c r="D1149" s="14"/>
@@ -6678,8 +6678,8 @@
       <c r="U1149" s="2"/>
       <c r="V1149" s="2"/>
     </row>
-    <row r="1152" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1155" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1152" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1155" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1155" s="14"/>
       <c r="B1155" s="7"/>
       <c r="C1155" s="12"/>
@@ -6703,7 +6703,7 @@
       <c r="U1155" s="2"/>
       <c r="V1155" s="2"/>
     </row>
-    <row r="1164" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1164" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1164" s="14"/>
       <c r="B1164" s="7"/>
       <c r="C1164" s="12"/>
@@ -6727,8 +6727,8 @@
       <c r="U1164" s="2"/>
       <c r="V1164" s="2"/>
     </row>
-    <row r="1165" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1166" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1165" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1166" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1166" s="14"/>
       <c r="B1166" s="7"/>
       <c r="C1166" s="12"/>
@@ -6752,7 +6752,7 @@
       <c r="U1166" s="2"/>
       <c r="V1166" s="2"/>
     </row>
-    <row r="1171" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1171" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1171" s="14"/>
       <c r="B1171" s="7"/>
       <c r="C1171" s="12"/>
@@ -6776,109 +6776,109 @@
       <c r="U1171" s="2"/>
       <c r="V1171" s="2"/>
     </row>
-    <row r="1174" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1181" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1210" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1211" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1212" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1213" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1214" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1215" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1216" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1217" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1218" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1219" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1220" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1221" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1222" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1223" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1224" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1225" ht="54.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1226" ht="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1227" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1228" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1229" ht="44.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1230" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1231" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1232" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1233" ht="30.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1234" ht="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1235" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1236" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1237" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1238" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1239" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1240" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1241" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1242" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1243" ht="45.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1244" ht="26.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1245" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1246" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1247" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1248" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1249" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1250" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1251" ht="37.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1252" ht="28.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1253" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1254" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1255" ht="25.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1256" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1257" ht="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1258" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1259" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1266" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1268" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1270" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1272" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1275" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1277" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1308" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1309" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1310" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1311" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1312" ht="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1313" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1314" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1315" ht="39.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1316" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1317" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1318" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1319" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1320" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1321" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1322" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1323" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1324" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1325" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1326" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1327" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1328" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1329" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1330" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1331" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1332" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1333" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1334" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1335" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1337" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1338" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1339" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1341" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1342" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1343" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1345" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1346" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1347" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1348" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1349" ht="44.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1350" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1351" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1352" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1353" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1366" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1174" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1181" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1195" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1210" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1211" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1212" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1213" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1214" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1215" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1216" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1217" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1218" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1219" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1220" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1221" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1222" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1223" ht="21.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1224" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1225" ht="54.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1226" ht="32.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1227" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1228" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1229" ht="44.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1230" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1231" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1232" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1233" ht="30.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1234" ht="33.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1235" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1236" ht="35.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1237" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1238" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1239" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1240" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1241" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1242" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1243" ht="45.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1244" ht="26.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1245" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1246" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1247" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1248" ht="23.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1249" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1250" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1251" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1252" ht="28.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1253" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1254" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1255" ht="25.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1256" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1257" ht="24.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1258" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1259" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1266" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1268" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1270" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1272" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1275" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1277" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1308" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1309" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1310" ht="41.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1311" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1312" ht="33.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1313" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1314" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1315" ht="39.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1316" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1317" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1318" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1319" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1320" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1321" ht="41.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1322" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1323" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1324" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1325" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1326" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1327" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1328" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1329" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1330" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1331" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1332" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1333" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1334" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1335" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1337" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1338" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1339" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1341" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1342" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1343" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1345" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1346" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1347" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1348" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1349" ht="44.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1350" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1351" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1352" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1353" ht="36" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1366" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -6902,7 +6902,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6916,7 +6916,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>